<commit_message>
initial commit of myths work under way
</commit_message>
<xml_diff>
--- a/data/atu/country_mapping.xlsx
+++ b/data/atu/country_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlg/Documents/Repos/_glos/data/atu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5822DDE5-789F-7E4E-9E95-6899B5172F73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F4C047C-4581-A84B-8968-BAAB4A881751}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="1000" windowWidth="27060" windowHeight="17400" xr2:uid="{A26192EF-B74F-1443-86C8-CDC8C1CA15E0}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6589" uniqueCount="4478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6589" uniqueCount="4479">
   <si>
     <t>Russia</t>
   </si>
@@ -13478,6 +13478,9 @@
   </si>
   <si>
     <t>Guyana, Suriname</t>
+  </si>
+  <si>
+    <t>geo_class</t>
   </si>
 </sst>
 </file>
@@ -13883,8 +13886,8 @@
   <dimension ref="A1:F224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C201" sqref="C201"/>
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -13903,7 +13906,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>4467</v>
+        <v>4478</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>4471</v>
@@ -16640,431 +16643,431 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>4341</v>
-      </c>
+        <v>4343</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D187" s="11"/>
       <c r="E187" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F187" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>161</v>
+        <v>342</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D188" s="11"/>
+        <v>4343</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>4476</v>
+      </c>
       <c r="E188" s="1" t="s">
-        <v>162</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>163</v>
+        <v>346</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D189" s="11"/>
+        <v>4343</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="E189" s="1" t="s">
-        <v>164</v>
+        <v>347</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>228</v>
+        <v>324</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>4341</v>
+        <v>4343</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>4475</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F190" s="5" t="s">
-        <v>4358</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>4341</v>
+        <v>4343</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>4310</v>
       </c>
       <c r="D191" s="11"/>
       <c r="E191" s="1" t="s">
-        <v>61</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>4341</v>
+        <v>4343</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D193" s="11"/>
+        <v>4343</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="E193" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F193" s="5" t="s">
-        <v>383</v>
+        <v>220</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>71</v>
+        <v>221</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D194" s="11"/>
+        <v>4343</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>375</v>
+      </c>
       <c r="E194" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F194" s="5" t="s">
-        <v>4368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>25</v>
+        <v>286</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>4341</v>
+        <v>4343</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="D195" s="11"/>
       <c r="E195" s="1" t="s">
-        <v>26</v>
+        <v>287</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D196" s="11"/>
+        <v>4343</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="E196" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F196" s="5" t="s">
-        <v>384</v>
+        <v>233</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>4341</v>
+        <v>4343</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>376</v>
       </c>
       <c r="D197" s="11"/>
       <c r="E197" s="1" t="s">
-        <v>171</v>
+        <v>376</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>104</v>
+        <v>175</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D198" s="11" t="s">
-        <v>4367</v>
+        <v>4343</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F198" s="5" t="s">
-        <v>4470</v>
+        <v>176</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>4341</v>
+        <v>4343</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>4363</v>
+        <v>260</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>4341</v>
-      </c>
-      <c r="D200" s="11"/>
+        <v>4343</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>4474</v>
+      </c>
       <c r="E200" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F200" s="5" t="s">
-        <v>387</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>168</v>
+        <v>325</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>4343</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D201" s="11"/>
+        <v>326</v>
+      </c>
       <c r="E201" s="1" t="s">
-        <v>374</v>
+        <v>326</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>342</v>
+        <v>297</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>4343</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>4476</v>
+        <v>4472</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>4476</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>346</v>
+        <v>284</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>4343</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>347</v>
+        <v>4473</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>347</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>324</v>
+        <v>237</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>4475</v>
+        <v>4341</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>4475</v>
+        <v>227</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>4310</v>
+        <v>4341</v>
       </c>
       <c r="D205" s="11"/>
       <c r="E205" s="1" t="s">
-        <v>4310</v>
+        <v>162</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>200</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D206" s="11"/>
       <c r="E206" s="1" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>220</v>
+        <v>4341</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>220</v>
+        <v>229</v>
+      </c>
+      <c r="F207" s="5" t="s">
+        <v>4358</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>221</v>
+        <v>60</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>375</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D208" s="11"/>
       <c r="E208" s="1" t="s">
-        <v>375</v>
+        <v>61</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>286</v>
+        <v>113</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D209" s="11"/>
+        <v>4341</v>
+      </c>
       <c r="E209" s="1" t="s">
-        <v>287</v>
+        <v>114</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>232</v>
+        <v>134</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D210" s="11"/>
       <c r="E210" s="1" t="s">
-        <v>233</v>
+        <v>135</v>
+      </c>
+      <c r="F210" s="5" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>222</v>
+        <v>71</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>376</v>
+        <v>4341</v>
       </c>
       <c r="D211" s="11"/>
       <c r="E211" s="1" t="s">
-        <v>376</v>
+        <v>72</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>4368</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>176</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D212" s="11"/>
       <c r="E212" s="1" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>217</v>
+        <v>261</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>218</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D213" s="11"/>
       <c r="E213" s="1" t="s">
-        <v>218</v>
+        <v>262</v>
+      </c>
+      <c r="F213" s="5" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>260</v>
+        <v>170</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>4474</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D214" s="11"/>
       <c r="E214" s="1" t="s">
-        <v>4474</v>
+        <v>171</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>325</v>
+        <v>104</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>326</v>
+        <v>4341</v>
+      </c>
+      <c r="D215" s="11" t="s">
+        <v>4367</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>326</v>
+        <v>3</v>
+      </c>
+      <c r="F215" s="5" t="s">
+        <v>4470</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>297</v>
+        <v>236</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>4472</v>
+        <v>4341</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>4472</v>
+        <v>227</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>284</v>
+        <v>4363</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>4473</v>
-      </c>
+        <v>4341</v>
+      </c>
+      <c r="D217" s="11"/>
       <c r="E217" s="1" t="s">
-        <v>4473</v>
+        <v>130</v>
+      </c>
+      <c r="F217" s="5" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>